<commit_message>
Fancy column enum (#22)
* fix review styles comments index and add tests
---------

Co-authored-by: Hazedd <hazzdd@no-replay.github.com>
</commit_message>
<xml_diff>
--- a/sample_data/issuelist-processed.xlsx
+++ b/sample_data/issuelist-processed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\IMX_dataverbetering\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5267923A-7409-4E85-BD1F-510B52F3390A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4503D3-D26B-4637-BF63-09A4A689BA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5475" yWindow="7350" windowWidth="43200" windowHeight="23445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process-log" sheetId="1" r:id="rId1"/>
@@ -4627,10 +4627,10 @@
     <t>value_new</t>
   </si>
   <si>
-    <t>processing_status</t>
-  </si>
-  <si>
     <t>revision_reasoning</t>
+  </si>
+  <si>
+    <t>will_be_processed</t>
   </si>
 </sst>
 </file>
@@ -5009,9 +5009,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1849"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5056,10 +5056,10 @@
         <v>1533</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>1535</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>1534</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>1535</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>0</v>

</xml_diff>